<commit_message>
Added more descriptive detail plus time to complete
</commit_message>
<xml_diff>
--- a/Admin/Jaco Engineparts Task List.xlsx
+++ b/Admin/Jaco Engineparts Task List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ep\Admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\GitHub\ep\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C86A16-CCC6-4C3E-8147-375E53DD11B7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="25320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="25320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Long term" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
   <si>
     <t>AEP Cataloguing Progress Report</t>
   </si>
@@ -36,9 +37,6 @@
   </si>
   <si>
     <t>Auto-Extract</t>
-  </si>
-  <si>
-    <t>Stock Reception History</t>
   </si>
   <si>
     <t>Samantha</t>
@@ -208,11 +206,104 @@
     <t>It's not stopping work, but it is a nuisance and a slight slowdown.
 I should check account AT4 to reproduce the problem.</t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Change code to add additional scanned pages. Ensure compatability to Builder C++ viewer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review duplicate price calc code needed to optimise reporting needs against real-time single item SP. </t>
+  </si>
+  <si>
+    <t>1st review indicated massive slow-down if single item SP used in bulk report.</t>
+  </si>
+  <si>
+    <t>Exclude specific SKU's from Optimiser</t>
+  </si>
+  <si>
+    <t>Extract SQL done, create SP &amp; Crystal report</t>
+  </si>
+  <si>
+    <t>2d</t>
+  </si>
+  <si>
+    <t>4d</t>
+  </si>
+  <si>
+    <t>Java Web based</t>
+  </si>
+  <si>
+    <t>Suspense GL Acc must = 0 &amp; is not</t>
+  </si>
+  <si>
+    <t>Review if still part of daily recon requirements against X3</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>Tomcat proxy server must be up &amp; running. Poor cust experience</t>
+  </si>
+  <si>
+    <t>Change C++ fat client loader, test &amp; monitor auto customer distribution</t>
+  </si>
+  <si>
+    <t>5d</t>
+  </si>
+  <si>
+    <t>Allow for load balancer of image &amp; exe distribution</t>
+  </si>
+  <si>
+    <t>6d</t>
+  </si>
+  <si>
+    <t>New development</t>
+  </si>
+  <si>
+    <t>Change frontend and test monotor functionality</t>
+  </si>
+  <si>
+    <t>Create a report with payment and other details - full lifecycle. Extract detail on demand only when paid for sale is returned / cancelled</t>
+  </si>
+  <si>
+    <t>Note: Payment &amp; monies returned can become complex - only report on activity without proposing how to conclude</t>
+  </si>
+  <si>
+    <t>Detail research needed</t>
+  </si>
+  <si>
+    <t>May require more time if difficult to find problem</t>
+  </si>
+  <si>
+    <t>1st Phase QlickView accepted positively
+Refinement being implemented
+Desktop installation to follow.
+Planning additional views and filters</t>
+  </si>
+  <si>
+    <t>Create summary of cashier shift for integration to X3. Change request received</t>
+  </si>
+  <si>
+    <t>Review requirement &amp; ascertain if granularity loss may create secondary issues</t>
+  </si>
+  <si>
+    <t>TBA</t>
+  </si>
+  <si>
+    <t>Stock Supplier Receipt History</t>
+  </si>
+  <si>
+    <t>Summary file to optimiza - daily schedule</t>
+  </si>
+  <si>
+    <t>Code completed, implement in schedular and monitor for correctness</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -538,11 +629,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,49 +641,53 @@
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="41.140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -600,10 +695,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="3">
         <v>43056</v>
@@ -611,8 +706,11 @@
       <c r="H2" s="1">
         <v>19296</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -620,10 +718,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3">
         <v>43056</v>
@@ -631,19 +729,25 @@
       <c r="H3" s="1">
         <v>19290</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="G4" s="3">
         <v>43059</v>
@@ -651,19 +755,28 @@
       <c r="H4" s="1">
         <v>19387</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="3">
         <v>43059</v>
@@ -671,19 +784,28 @@
       <c r="H5" s="1">
         <v>19389</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="3">
         <v>43059</v>
@@ -691,19 +813,28 @@
       <c r="H6" s="1">
         <v>19390</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="3">
         <v>43131</v>
@@ -711,19 +842,28 @@
       <c r="H7" s="1">
         <v>25365</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3">
         <v>43046</v>
@@ -731,56 +871,80 @@
       <c r="H8" s="1">
         <v>25872</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="G9" s="3">
         <v>43426</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="G10" s="3">
         <v>43426</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="G11" s="3">
         <v>43173</v>
@@ -788,19 +952,25 @@
       <c r="H11" s="1">
         <v>29497</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" s="3">
         <v>43293</v>
@@ -808,19 +978,22 @@
       <c r="H12" s="1">
         <v>43714</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G13" s="3">
         <v>43382</v>
@@ -828,19 +1001,28 @@
       <c r="H13" s="1">
         <v>67452</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="G14" s="3">
         <v>43389</v>
@@ -848,19 +1030,28 @@
       <c r="H14" s="1">
         <v>69325</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
+      <c r="D15" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15" s="3">
         <v>43392</v>
@@ -868,19 +1059,25 @@
       <c r="H15" s="1">
         <v>71665</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="G16" s="3">
         <v>43398</v>
@@ -888,19 +1085,25 @@
       <c r="H16" s="1">
         <v>73102</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="G17" s="3">
         <v>43412</v>
@@ -908,25 +1111,31 @@
       <c r="H17" s="1">
         <v>76573</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="J17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="G18" s="3">
         <v>43419</v>
@@ -935,30 +1144,36 @@
         <v>43425</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G19" s="3">
         <v>43426</v>
       </c>
       <c r="H19" s="1">
         <v>81577</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>